<commit_message>
Updated to make sure graphs were correct.
</commit_message>
<xml_diff>
--- a/Results/allCombo.xlsx
+++ b/Results/allCombo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8655" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8655"/>
   </bookViews>
   <sheets>
     <sheet name="Ubuntu" sheetId="1" r:id="rId1"/>
@@ -154,6 +154,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Ubuntu Mate</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> - All Average vs. Middle 31 Average</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -898,6 +928,8 @@
         <c:axId val="636319592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="2.1"/>
+          <c:min val="0.9"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1110,6 +1142,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Ubuntu Mate</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1417,6 +1474,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Raspbian - All Average vs. Middle 31 Average</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1431,7 +1513,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2161,6 +2243,7 @@
         <c:axId val="392073648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.9"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2200,7 +2283,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2240,6 +2323,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2262,7 +2401,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2305,7 +2444,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2345,7 +2484,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1200"/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -2373,6 +2512,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Raspbian</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -2387,7 +2551,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2542,7 +2706,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2601,7 +2765,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2652,7 +2816,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1200"/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -2680,6 +2844,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Arch Linux - All Average vs Middle 26 Average </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -2694,7 +2883,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2854,7 +3043,7 @@
                   <c:v>37442.074999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37453.5</c:v>
+                  <c:v>37441.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2929,7 +3118,7 @@
                   <c:v>37460</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37459.800000000003</c:v>
+                  <c:v>37458.576923076922</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3004,7 +3193,7 @@
                   <c:v>37432.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37425.833333333336</c:v>
+                  <c:v>37434.038461538461</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3079,7 +3268,7 @@
                   <c:v>37438</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37446.160000000003</c:v>
+                  <c:v>37444.961538461539</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3154,7 +3343,7 @@
                   <c:v>37530.117647058825</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37548.192307692305</c:v>
+                  <c:v>37548.653846153844</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3316,7 +3505,7 @@
                   <c:v>37438.93548387097</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37436.080000000002</c:v>
+                  <c:v>37436.115384615383</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3397,7 +3586,7 @@
                   <c:v>37550.205882352944</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37550.925925925927</c:v>
+                  <c:v>37549.269230769234</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3424,6 +3613,7 @@
         <c:axId val="392063808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.9"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -3463,7 +3653,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3525,7 +3715,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3568,7 +3758,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -3608,7 +3798,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1200"/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -3636,6 +3826,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Arch Linux</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -3650,7 +3865,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -3731,28 +3946,28 @@
                   <c:v>37576.730769230766</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37453.5</c:v>
+                  <c:v>37441.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>37459.800000000003</c:v>
+                  <c:v>37458.576923076922</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37425.833333333336</c:v>
+                  <c:v>37434.038461538461</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37446.160000000003</c:v>
+                  <c:v>37444.961538461539</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37548.192307692305</c:v>
+                  <c:v>37548.653846153844</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>37409.599999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>37436.080000000002</c:v>
+                  <c:v>37436.115384615383</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>37550.925925925927</c:v>
+                  <c:v>37549.269230769234</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3805,7 +4020,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3855,7 +4070,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -3888,7 +4103,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -3920,7 +4135,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3971,7 +4186,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1200"/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -4640,28 +4855,28 @@
                   <c:v>37576.730769230766</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37453.5</c:v>
+                  <c:v>37441.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>37459.800000000003</c:v>
+                  <c:v>37458.576923076922</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37425.833333333336</c:v>
+                  <c:v>37434.038461538461</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37446.160000000003</c:v>
+                  <c:v>37444.961538461539</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37548.192307692305</c:v>
+                  <c:v>37548.653846153844</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>37409.599999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>37436.080000000002</c:v>
+                  <c:v>37436.115384615383</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>37550.925925925927</c:v>
+                  <c:v>37549.269230769234</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9271,16 +9486,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>513849</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>157413</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>577091</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>128298</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>159585</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>66842</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>81752</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>35220</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9301,16 +9516,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>145382</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>176211</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>593616</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>142592</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>418599</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>99510</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>549087</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>11205</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9337,13 +9552,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>224203</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>25154</xdr:rowOff>
+      <xdr:colOff>224204</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>136071</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>136770</xdr:colOff>
+      <xdr:colOff>176892</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>146538</xdr:rowOff>
     </xdr:to>
@@ -9366,16 +9581,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>542192</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>297264</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>159726</xdr:rowOff>
+      <xdr:rowOff>50869</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>45426</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>176892</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>136071</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9408,7 +9623,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>311728</xdr:colOff>
+      <xdr:colOff>476250</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>167407</xdr:rowOff>
     </xdr:to>
@@ -9792,8 +10007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView zoomScale="76" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11424,8 +11639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView zoomScale="65" workbookViewId="0">
-      <selection activeCell="B1" activeCellId="1" sqref="B54:J54 B1:J1"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12949,8 +13164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="AH31" sqref="AH31"/>
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14237,36 +14452,36 @@
         <v>37576.730769230766</v>
       </c>
       <c r="C54">
-        <f>AVERAGE(C8:C33)</f>
-        <v>37453.5</v>
+        <f>AVERAGE(C9:C33)</f>
+        <v>37441.4</v>
       </c>
       <c r="D54">
-        <f>AVERAGE(D6:D30)</f>
-        <v>37459.800000000003</v>
+        <f>AVERAGE(D6:D31)</f>
+        <v>37458.576923076922</v>
       </c>
       <c r="E54">
-        <f>AVERAGE(E6:E29)</f>
-        <v>37425.833333333336</v>
+        <f>AVERAGE(E5:E30)</f>
+        <v>37434.038461538461</v>
       </c>
       <c r="F54">
-        <f>AVERAGE(F6:F30)</f>
-        <v>37446.160000000003</v>
+        <f>AVERAGE(F5:F30)</f>
+        <v>37444.961538461539</v>
       </c>
       <c r="G54">
-        <f>AVERAGE(G6:G31)</f>
-        <v>37548.192307692305</v>
+        <f>AVERAGE(G13:G38)</f>
+        <v>37548.653846153844</v>
       </c>
       <c r="H54">
         <f>AVERAGE(H6:H30)</f>
         <v>37409.599999999999</v>
       </c>
       <c r="I54">
-        <f>AVERAGE(I5:I29)</f>
-        <v>37436.080000000002</v>
+        <f>AVERAGE(I5:I30)</f>
+        <v>37436.115384615383</v>
       </c>
       <c r="J54">
-        <f>AVERAGE(J6:J32)</f>
-        <v>37550.925925925927</v>
+        <f>AVERAGE(J6:J31)</f>
+        <v>37549.269230769234</v>
       </c>
     </row>
   </sheetData>
@@ -14279,7 +14494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="L57" sqref="L57"/>
     </sheetView>
   </sheetViews>
@@ -14409,23 +14624,23 @@
       </c>
       <c r="C4">
         <f>Arch!C54</f>
-        <v>37453.5</v>
+        <v>37441.4</v>
       </c>
       <c r="D4">
         <f>Arch!D54</f>
-        <v>37459.800000000003</v>
+        <v>37458.576923076922</v>
       </c>
       <c r="E4">
         <f>Arch!E54</f>
-        <v>37425.833333333336</v>
+        <v>37434.038461538461</v>
       </c>
       <c r="F4">
         <f>Arch!F54</f>
-        <v>37446.160000000003</v>
+        <v>37444.961538461539</v>
       </c>
       <c r="G4">
         <f>Arch!G54</f>
-        <v>37548.192307692305</v>
+        <v>37548.653846153844</v>
       </c>
       <c r="H4">
         <f>Arch!H54</f>
@@ -14433,11 +14648,11 @@
       </c>
       <c r="I4">
         <f>Arch!I54</f>
-        <v>37436.080000000002</v>
+        <v>37436.115384615383</v>
       </c>
       <c r="J4">
         <f>Arch!J54</f>
-        <v>37550.925925925927</v>
+        <v>37549.269230769234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>